<commit_message>
maj du fichier Excel avec cellules nommées et tableau
</commit_message>
<xml_diff>
--- a/AlarmeTests.xlsx
+++ b/AlarmeTests.xlsx
@@ -8,13 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OD\420-6J5 Prog1\Cours\Cours 11 Conditions composées\2 Exercices série 5\SolutionsSérie5\5.5_alarme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F411E23-CB9C-43E2-922F-62698BF188AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DBEBB7-E897-46E1-BEBF-78D5B6659811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DA04357E-3799-430A-8FD2-3DEDAABA1FC4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{DA04357E-3799-430A-8FD2-3DEDAABA1FC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="ARMÉ">Sheet1!$A$1</definedName>
+    <definedName name="fenêtre_ouverte">Sheet1!$D$1</definedName>
+    <definedName name="mouvement">Sheet1!$E$1</definedName>
+    <definedName name="portes_verrouillées">Sheet1!$C$1</definedName>
+    <definedName name="PRÉSENT">Sheet1!$B$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,9 +51,6 @@
     <t>PRÉSENT</t>
   </si>
   <si>
-    <t>porte_verrouillées</t>
-  </si>
-  <si>
     <t>fenêtre_ouverte</t>
   </si>
   <si>
@@ -54,6 +58,9 @@
   </si>
   <si>
     <t>résultat alarme</t>
+  </si>
+  <si>
+    <t>portes_verrouillées</t>
   </si>
 </sst>
 </file>
@@ -110,7 +117,11 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -121,6 +132,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AAE4A7FD-F085-48B7-82AE-65BC2FA19753}" name="Table1" displayName="Table1" ref="A1:F33" totalsRowShown="0">
+  <autoFilter ref="A1:F33" xr:uid="{AAE4A7FD-F085-48B7-82AE-65BC2FA19753}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{40D716BE-2D1D-476E-B163-953C130BEF1E}" name="ARMÉ"/>
+    <tableColumn id="2" xr3:uid="{9E33591B-FF72-4E9F-8167-8D0179D9EC00}" name="PRÉSENT"/>
+    <tableColumn id="3" xr3:uid="{F20B8594-6485-49E9-99E5-EE527F752A03}" name="portes_verrouillées"/>
+    <tableColumn id="4" xr3:uid="{F061FF89-F57E-40B9-AEC4-0875B2DF5DF0}" name="fenêtre_ouverte"/>
+    <tableColumn id="5" xr3:uid="{42DD1920-2F96-4A9C-B12A-00D0104F1CF2}" name="mouvement"/>
+    <tableColumn id="6" xr3:uid="{14893AB6-5C2E-458C-83EE-81EA7E23C15E}" name="résultat alarme" dataDxfId="0" dataCellStyle="Good">
+      <calculatedColumnFormula>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -444,15 +472,16 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="14.109375" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -463,16 +492,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -492,7 +521,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="b">
-        <f>AND(A2, OR(NOT(C2), AND(NOT(B2), OR(D2,E2))))</f>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>0</v>
       </c>
     </row>
@@ -513,7 +542,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="1" t="b">
-        <f t="shared" ref="F3:F33" si="0">AND(A3, OR(NOT(C3), AND(NOT(B3), OR(D3,E3))))</f>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>0</v>
       </c>
     </row>
@@ -534,7 +563,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>0</v>
       </c>
     </row>
@@ -555,7 +584,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>0</v>
       </c>
     </row>
@@ -576,7 +605,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>1</v>
       </c>
     </row>
@@ -597,7 +626,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>1</v>
       </c>
     </row>
@@ -618,7 +647,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>1</v>
       </c>
     </row>
@@ -639,7 +668,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>1</v>
       </c>
     </row>
@@ -660,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>1</v>
       </c>
     </row>
@@ -681,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>1</v>
       </c>
     </row>
@@ -702,7 +731,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>1</v>
       </c>
     </row>
@@ -723,7 +752,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>0</v>
       </c>
     </row>
@@ -744,7 +773,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>1</v>
       </c>
     </row>
@@ -765,7 +794,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>1</v>
       </c>
     </row>
@@ -786,7 +815,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>1</v>
       </c>
     </row>
@@ -807,7 +836,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>1</v>
       </c>
     </row>
@@ -828,7 +857,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>0</v>
       </c>
     </row>
@@ -849,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>0</v>
       </c>
     </row>
@@ -870,7 +899,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>0</v>
       </c>
     </row>
@@ -891,7 +920,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>0</v>
       </c>
     </row>
@@ -912,7 +941,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>0</v>
       </c>
     </row>
@@ -933,7 +962,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>0</v>
       </c>
     </row>
@@ -954,7 +983,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>0</v>
       </c>
     </row>
@@ -975,7 +1004,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>0</v>
       </c>
     </row>
@@ -996,7 +1025,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>0</v>
       </c>
     </row>
@@ -1017,7 +1046,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>0</v>
       </c>
     </row>
@@ -1038,7 +1067,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>0</v>
       </c>
     </row>
@@ -1059,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>0</v>
       </c>
     </row>
@@ -1080,7 +1109,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>0</v>
       </c>
     </row>
@@ -1101,7 +1130,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>0</v>
       </c>
     </row>
@@ -1122,7 +1151,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>0</v>
       </c>
     </row>
@@ -1143,11 +1172,14 @@
         <v>0</v>
       </c>
       <c r="F33" s="1" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(Table1[[#This Row],[ARMÉ]], OR(NOT(Table1[[#This Row],[portes_verrouillées]]), AND(NOT(Table1[[#This Row],[PRÉSENT]]), OR(Table1[[#This Row],[fenêtre_ouverte]],Table1[[#This Row],[mouvement]]))))</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>